<commit_message>
Added storageBenchmarker, restrucured even further
git-svn-id: https://svnserver.informatik.kit.edu/i43/svn/code@4806 769cc9a0-fb0c-0410-8c2f-a2305f0e6268
</commit_message>
<xml_diff>
--- a/FileShare/learningInputData/InprecisionTracing.xlsx
+++ b/FileShare/learningInputData/InprecisionTracing.xlsx
@@ -7,10 +7,13 @@
     <workbookView xWindow="360" yWindow="75" windowWidth="17040" windowHeight="12345"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Lenovo" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Lenovo!$A$1:$L$28</definedName>
+  </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
@@ -182,9 +185,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
-    <numFmt numFmtId="168" formatCode="#,##0.0000"/>
-    <numFmt numFmtId="169" formatCode="0.0000"/>
-    <numFmt numFmtId="170" formatCode="#,##0.000"/>
+    <numFmt numFmtId="164" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="#,##0.000"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -401,10 +404,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -413,19 +416,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -434,37 +437,37 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="6" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="6" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="170" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -534,7 +537,7 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$21</c:f>
+              <c:f>Lenovo!$A$2:$A$21</c:f>
               <c:strCache>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
@@ -602,7 +605,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$2:$H$21</c:f>
+              <c:f>Lenovo!$H$2:$H$21</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.0000</c:formatCode>
                 <c:ptCount val="20"/>
@@ -670,24 +673,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="54203904"/>
-        <c:axId val="54205824"/>
+        <c:axId val="80253312"/>
+        <c:axId val="80254848"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="54203904"/>
+        <c:axId val="80253312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="54205824"/>
+        <c:crossAx val="80254848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="54205824"/>
+        <c:axId val="80254848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -695,7 +698,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="#,##0.0000" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="54203904"/>
+        <c:crossAx val="80253312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -704,7 +707,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -730,7 +733,7 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$21</c:f>
+              <c:f>Lenovo!$A$2:$A$21</c:f>
               <c:strCache>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
@@ -798,7 +801,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$K$2:$K$21</c:f>
+              <c:f>Lenovo!$K$2:$K$21</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="20"/>
@@ -866,24 +869,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="61666048"/>
-        <c:axId val="61667584"/>
+        <c:axId val="80643584"/>
+        <c:axId val="80645120"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="61666048"/>
+        <c:axId val="80643584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61667584"/>
+        <c:crossAx val="80645120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="61667584"/>
+        <c:axId val="80645120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -891,7 +894,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61666048"/>
+        <c:crossAx val="80643584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -900,7 +903,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -922,7 +925,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$L$1</c:f>
+              <c:f>Lenovo!$L$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -933,7 +936,7 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$21</c:f>
+              <c:f>Lenovo!$A$2:$A$21</c:f>
               <c:strCache>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
@@ -1001,7 +1004,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$L$2:$L$21</c:f>
+              <c:f>Lenovo!$L$2:$L$21</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.000</c:formatCode>
                 <c:ptCount val="20"/>
@@ -1070,24 +1073,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="110560384"/>
-        <c:axId val="110561920"/>
+        <c:axId val="80664832"/>
+        <c:axId val="80871424"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="110560384"/>
+        <c:axId val="80664832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110561920"/>
+        <c:crossAx val="80871424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="110561920"/>
+        <c:axId val="80871424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1095,7 +1098,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="#,##0.000" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110560384"/>
+        <c:crossAx val="80664832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1104,7 +1107,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -1493,7 +1496,7 @@
   <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection sqref="A1:L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1512,7 +1515,7 @@
     <col min="257" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="75">
+    <row r="1" spans="1:12" ht="90">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
@@ -1620,7 +1623,7 @@
         <v>0.64894678926838401</v>
       </c>
       <c r="I3" s="16">
-        <f t="shared" ref="I3:J21" si="1">G3/$H$23</f>
+        <f t="shared" ref="I3:I21" si="1">G3/$H$23</f>
         <v>6978490284.0278406</v>
       </c>
       <c r="J3" s="23">

</xml_diff>